<commit_message>
can deal with different sbol object types
can now make experiments etc. Can lookup values in a list. sequence, circular, and data source have been updated.
</commit_message>
<xml_diff>
--- a/excel2sbol/tests/test_files/pichia_tyto.xlsx
+++ b/excel2sbol/tests/test_files/pichia_tyto.xlsx
@@ -8,14 +8,16 @@
   </bookViews>
   <sheets>
     <sheet name="Library" sheetId="1" r:id="rId1"/>
-    <sheet name="role_terms" sheetId="2" r:id="rId2"/>
-    <sheet name="Organism Terms" sheetId="3" r:id="rId3"/>
-    <sheet name="Sequence_alteration_terms" sheetId="4" r:id="rId4"/>
-    <sheet name="data_source" sheetId="5" r:id="rId5"/>
-    <sheet name="column_definitions" sheetId="6" r:id="rId6"/>
+    <sheet name="Object_Types" sheetId="7" r:id="rId2"/>
+    <sheet name="circular_types" sheetId="8" r:id="rId3"/>
+    <sheet name="role_terms" sheetId="2" r:id="rId4"/>
+    <sheet name="Organism Terms" sheetId="3" r:id="rId5"/>
+    <sheet name="Sequence_alteration_terms" sheetId="4" r:id="rId6"/>
+    <sheet name="data_source" sheetId="5" r:id="rId7"/>
+    <sheet name="column_definitions" sheetId="6" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">role_terms!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">role_terms!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7795" uniqueCount="7627">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7877" uniqueCount="7664">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22631,15 +22633,9 @@
     <t>https://pubmed.ncbi.nlm.nih.gov</t>
   </si>
   <si>
-    <t>https://pubmed.ncbi.nlm.nih.gov/24295448/</t>
-  </si>
-  <si>
     <t>PMID:24295448</t>
   </si>
   <si>
-    <t>https://pubmed.ncbi.nlm.nih.gov/{REPLACE_HERE}/</t>
-  </si>
-  <si>
     <t>iGEM</t>
   </si>
   <si>
@@ -22667,15 +22663,9 @@
     <t>https://www.addgene.org</t>
   </si>
   <si>
-    <t>https://www.addgene.org/87906/</t>
-  </si>
-  <si>
     <t>AG:87906</t>
   </si>
   <si>
-    <t>https://www.addgene.org/{REPLACE_HERE}/</t>
-  </si>
-  <si>
     <t>Seva plasmids</t>
   </si>
   <si>
@@ -22764,9 +22754,6 @@
   </si>
   <si>
     <t>sbh_targetOrganism</t>
-  </si>
-  <si>
-    <t>sbol_roleCircular</t>
   </si>
   <si>
     <t>sbol_sequence</t>
@@ -22971,6 +22958,9 @@
     <t>sbh_splitTest</t>
   </si>
   <si>
+    <t>":"</t>
+  </si>
+  <si>
     <t>":""_"</t>
   </si>
   <si>
@@ -22984,13 +22974,156 @@
   </si>
   <si>
     <t>again_hi</t>
+  </si>
+  <si>
+    <t>SBOL Object Type</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>sbol_objectType</t>
+  </si>
+  <si>
+    <t>ComponentDefinition</t>
+  </si>
+  <si>
+    <t>Activity</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Agent</t>
+  </si>
+  <si>
+    <t>Association</t>
+  </si>
+  <si>
+    <t>Attachment</t>
+  </si>
+  <si>
+    <t>Collection</t>
+  </si>
+  <si>
+    <t>CombinatorialDerivation</t>
+  </si>
+  <si>
+    <t>Cut</t>
+  </si>
+  <si>
+    <t>Experiment</t>
+  </si>
+  <si>
+    <t>ExperimentalData</t>
+  </si>
+  <si>
+    <t>FunctionalComponent</t>
+  </si>
+  <si>
+    <t>GenericLocation</t>
+  </si>
+  <si>
+    <t>Implementation</t>
+  </si>
+  <si>
+    <t>Interaction</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>MapsTo</t>
+  </si>
+  <si>
+    <t>Measure</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>ModuleDefinition</t>
+  </si>
+  <si>
+    <t>Participation</t>
+  </si>
+  <si>
+    <t>Plan</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>SequenceAnnotation</t>
+  </si>
+  <si>
+    <t>SequenceConstraint</t>
+  </si>
+  <si>
+    <t>Usage</t>
+  </si>
+  <si>
+    <t>VariableComponent</t>
+  </si>
+  <si>
+    <t>SBOL Object Types</t>
+  </si>
+  <si>
+    <r>
+      <t>"^[a-zA-Z \s*]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFD4D4D4"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>$" "https:\/\/www.ncbi.nlm.nih.gov/nuccore/.*"</t>
+    </r>
+  </si>
+  <si>
+    <t>promoter:CDS</t>
+  </si>
+  <si>
+    <t>Conversion</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/SO_0000988</t>
+  </si>
+  <si>
+    <t>circular_types</t>
+  </si>
+  <si>
+    <t>https://www.addgene.org/87906</t>
+  </si>
+  <si>
+    <t>https://www.addgene.org/{REPLACE_HERE}</t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/{REPLACE_HERE}</t>
+  </si>
+  <si>
+    <t>https://pubmed.ncbi.nlm.nih.gov/24295448</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -23138,6 +23271,14 @@
     <font>
       <sz val="12"/>
       <color rgb="FFD4D4D4"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -23327,7 +23468,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="5" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -23366,6 +23507,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="5" borderId="12" xfId="2"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="11" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -23377,7 +23523,27 @@
     <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="7">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -23439,9 +23605,9 @@
   </dxfs>
   <tableStyles count="1">
     <tableStyle name="Library-style" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="4"/>
-      <tableStyleElement type="firstRowStripe" dxfId="3"/>
-      <tableStyleElement type="secondRowStripe" dxfId="2"/>
+      <tableStyleElement type="headerRow" dxfId="6"/>
+      <tableStyleElement type="firstRowStripe" dxfId="5"/>
+      <tableStyleElement type="secondRowStripe" dxfId="4"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -23456,17 +23622,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A19:O40">
-  <tableColumns count="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="A19:P40">
+  <tableColumns count="16">
     <tableColumn id="1" name="Part Name"/>
+    <tableColumn id="16" name="SBOL Object Type" dataDxfId="3"/>
     <tableColumn id="2" name="Role"/>
-    <tableColumn id="15" name="Thing2" dataDxfId="0"/>
+    <tableColumn id="15" name="Thing2" dataDxfId="2"/>
     <tableColumn id="14" name="Thing1" dataDxfId="1"/>
     <tableColumn id="3" name="Design Notes"/>
     <tableColumn id="4" name="Altered Sequence"/>
     <tableColumn id="5" name="Part Description"/>
     <tableColumn id="6" name="Data Source Prefix"/>
-    <tableColumn id="7" name="Data Source"/>
+    <tableColumn id="7" name="Data Source" dataDxfId="0" dataCellStyle="Normal"/>
     <tableColumn id="8" name="Source Organism"/>
     <tableColumn id="9" name="Target Organism"/>
     <tableColumn id="10" name="Circular"/>
@@ -23676,10 +23843,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB96"/>
+  <dimension ref="A1:AC96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3046875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -23693,7 +23860,7 @@
     <col min="7" max="7" width="14.3046875" customWidth="1"/>
     <col min="8" max="8" width="13.84375" customWidth="1"/>
     <col min="9" max="9" width="15.53515625" customWidth="1"/>
-    <col min="10" max="10" width="8.3828125" customWidth="1"/>
+    <col min="10" max="10" width="14.4609375" customWidth="1"/>
     <col min="11" max="26" width="8.53515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -23810,12 +23977,12 @@
       <c r="J10" s="3"/>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="38"/>
-      <c r="B11" s="39"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="40"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="44"/>
+      <c r="F11" s="45"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
@@ -23977,7 +24144,7 @@
       <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
     </row>
-    <row r="17" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="13" t="s">
         <v>22</v>
       </c>
@@ -24009,7 +24176,7 @@
       <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
     </row>
-    <row r="18" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>24</v>
       </c>
@@ -24050,149 +24217,155 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="18" t="s">
         <v>37</v>
       </c>
       <c r="B19" s="18" t="s">
+        <v>7623</v>
+      </c>
+      <c r="C19" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="18" t="s">
-        <v>7624</v>
-      </c>
       <c r="D19" s="18" t="s">
-        <v>7619</v>
-      </c>
-      <c r="E19" s="19" t="s">
+        <v>7620</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>7614</v>
+      </c>
+      <c r="F19" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="F19" s="18" t="s">
+      <c r="G19" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="G19" s="19" t="s">
+      <c r="H19" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="H19" s="19" t="s">
+      <c r="I19" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="I19" s="19" t="s">
+      <c r="J19" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="J19" s="18" t="s">
+      <c r="K19" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="K19" s="18" t="s">
+      <c r="L19" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="L19" s="18" t="s">
+      <c r="M19" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="M19" s="18" t="s">
+      <c r="N19" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="N19" s="18" t="s">
+      <c r="O19" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="O19" s="18" t="s">
+      <c r="P19" s="18" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="20" t="s">
         <v>50</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>7625</v>
-      </c>
+        <v>7635</v>
+      </c>
+      <c r="C20" s="20"/>
       <c r="D20" s="20" t="s">
-        <v>7620</v>
-      </c>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20" t="s">
+        <v>7621</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>7615</v>
+      </c>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="20" t="s">
+      <c r="H20" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="H20" s="20" t="s">
+      <c r="I20" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="I20" s="20">
+      <c r="J20" s="38">
         <v>28252957</v>
       </c>
-      <c r="J20" t="s">
-        <v>7578</v>
-      </c>
       <c r="K20" t="s">
-        <v>7578</v>
-      </c>
-      <c r="L20" s="20" t="b">
+        <v>7573</v>
+      </c>
+      <c r="L20" t="s">
+        <v>7573</v>
+      </c>
+      <c r="M20" s="20" t="b">
         <v>0</v>
       </c>
-      <c r="M20" s="18">
-        <f t="shared" ref="M20:M40" si="0">LEN(SUBSTITUTE(N20," ",""))</f>
+      <c r="N20" s="18">
+        <f t="shared" ref="N20:N40" si="0">LEN(SUBSTITUTE(O20," ",""))</f>
         <v>939</v>
       </c>
-      <c r="N20" s="20" t="s">
+      <c r="O20" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="O20" s="18" t="str">
-        <f>Library!$H20&amp;":"&amp;Library!$I20</f>
+      <c r="P20" s="18" t="str">
+        <f>Library!$I20&amp;":"&amp;Library!$J20</f>
         <v>PubMed:28252957</v>
       </c>
     </row>
-    <row r="21" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="20" t="s">
         <v>56</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>51</v>
+        <v>7626</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>7626</v>
+        <v>7656</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>7623</v>
+        <v>7622</v>
       </c>
       <c r="E21" s="20" t="s">
+        <v>7619</v>
+      </c>
+      <c r="F21" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="F21" s="20" t="s">
+      <c r="G21" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="G21" s="20" t="s">
+      <c r="H21" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="H21" s="20" t="s">
+      <c r="I21" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="I21" s="20">
+      <c r="J21" s="38">
         <v>28252957</v>
       </c>
-      <c r="J21" t="s">
-        <v>7578</v>
-      </c>
       <c r="K21" t="s">
-        <v>7578</v>
-      </c>
-      <c r="L21" s="20" t="b">
+        <v>7573</v>
+      </c>
+      <c r="L21" t="s">
+        <v>7573</v>
+      </c>
+      <c r="M21" s="20" t="b">
         <v>0</v>
       </c>
-      <c r="M21" s="18">
+      <c r="N21" s="18">
         <f t="shared" si="0"/>
         <v>477</v>
       </c>
-      <c r="N21" s="20" t="s">
+      <c r="O21" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="O21" s="18" t="str">
-        <f>Library!$H21&amp;":"&amp;Library!$I21</f>
+      <c r="P21" s="18" t="str">
+        <f>Library!$I21&amp;":"&amp;Library!$J21</f>
         <v>PubMed:28252957</v>
       </c>
-      <c r="P21" s="3"/>
       <c r="Q21" s="3"/>
       <c r="R21" s="3"/>
       <c r="S21" s="3"/>
@@ -24205,52 +24378,55 @@
       <c r="Z21" s="3"/>
       <c r="AA21" s="3"/>
       <c r="AB21" s="3"/>
-    </row>
-    <row r="22" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AC21" s="3"/>
+    </row>
+    <row r="22" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="20" t="s">
         <v>61</v>
       </c>
       <c r="B22" s="20" t="s">
+        <v>7626</v>
+      </c>
+      <c r="C22" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="20"/>
       <c r="D22" s="20"/>
-      <c r="E22" s="20" t="s">
+      <c r="E22" s="20"/>
+      <c r="F22" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="F22" s="20" t="s">
+      <c r="G22" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="G22" s="20" t="s">
+      <c r="H22" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="H22" s="20" t="s">
+      <c r="I22" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="I22" s="20">
+      <c r="J22" s="38">
         <v>28252957</v>
       </c>
-      <c r="J22" s="33" t="s">
+      <c r="K22" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="K22" t="s">
-        <v>7578</v>
-      </c>
-      <c r="L22" s="20" t="b">
+      <c r="L22" t="s">
+        <v>7573</v>
+      </c>
+      <c r="M22" s="20" t="b">
         <v>0</v>
       </c>
-      <c r="M22" s="18">
+      <c r="N22" s="18">
         <f t="shared" si="0"/>
         <v>998</v>
       </c>
-      <c r="N22" s="20" t="s">
+      <c r="O22" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="O22" s="18" t="str">
-        <f>Library!$H22&amp;":"&amp;Library!$I22</f>
+      <c r="P22" s="18" t="str">
+        <f>Library!$I22&amp;":"&amp;Library!$J22</f>
         <v>PubMed:28252957</v>
       </c>
-      <c r="P22" s="3"/>
       <c r="Q22" s="3"/>
       <c r="R22" s="3"/>
       <c r="S22" s="3"/>
@@ -24263,50 +24439,53 @@
       <c r="Z22" s="3"/>
       <c r="AA22" s="3"/>
       <c r="AB22" s="3"/>
-    </row>
-    <row r="23" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AC22" s="3"/>
+    </row>
+    <row r="23" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="20" t="s">
         <v>66</v>
       </c>
       <c r="B23" s="20" t="s">
+        <v>7626</v>
+      </c>
+      <c r="C23" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="20"/>
       <c r="D23" s="20"/>
       <c r="E23" s="20"/>
-      <c r="F23" s="20" t="s">
+      <c r="F23" s="20"/>
+      <c r="G23" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="G23" s="20" t="s">
+      <c r="H23" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="H23" s="20" t="s">
+      <c r="I23" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="I23" s="20">
+      <c r="J23" s="38">
         <v>28252957</v>
       </c>
-      <c r="J23" s="20" t="s">
+      <c r="K23" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="K23" t="s">
-        <v>7578</v>
-      </c>
-      <c r="L23" s="20" t="b">
+      <c r="L23" t="s">
+        <v>7573</v>
+      </c>
+      <c r="M23" s="20" t="b">
         <v>0</v>
       </c>
-      <c r="M23" s="18">
+      <c r="N23" s="18">
         <f t="shared" si="0"/>
         <v>584</v>
       </c>
-      <c r="N23" s="20" t="s">
+      <c r="O23" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="O23" s="18" t="str">
-        <f>Library!$H23&amp;":"&amp;Library!$I23</f>
+      <c r="P23" s="18" t="str">
+        <f>Library!$I23&amp;":"&amp;Library!$J23</f>
         <v>PubMed:28252957</v>
       </c>
-      <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
       <c r="R23" s="3"/>
       <c r="S23" s="3"/>
@@ -24319,50 +24498,53 @@
       <c r="Z23" s="3"/>
       <c r="AA23" s="3"/>
       <c r="AB23" s="3"/>
-    </row>
-    <row r="24" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AC23" s="3"/>
+    </row>
+    <row r="24" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="20" t="s">
         <v>69</v>
       </c>
       <c r="B24" s="20" t="s">
+        <v>7626</v>
+      </c>
+      <c r="C24" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="C24" s="20"/>
       <c r="D24" s="20"/>
       <c r="E24" s="20"/>
-      <c r="F24" s="20" t="s">
+      <c r="F24" s="20"/>
+      <c r="G24" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="G24" s="20" t="s">
+      <c r="H24" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="H24" s="20" t="s">
+      <c r="I24" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="I24" s="20">
+      <c r="J24" s="38">
         <v>28252957</v>
       </c>
-      <c r="J24" s="20" t="s">
+      <c r="K24" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="K24" t="s">
-        <v>7578</v>
-      </c>
-      <c r="L24" s="20" t="b">
+      <c r="L24" t="s">
+        <v>7573</v>
+      </c>
+      <c r="M24" s="20" t="b">
         <v>0</v>
       </c>
-      <c r="M24" s="18">
+      <c r="N24" s="18">
         <f t="shared" si="0"/>
         <v>267</v>
       </c>
-      <c r="N24" s="20" t="s">
+      <c r="O24" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="O24" s="18" t="str">
-        <f>Library!$H24&amp;":"&amp;Library!$I24</f>
+      <c r="P24" s="18" t="str">
+        <f>Library!$I24&amp;":"&amp;Library!$J24</f>
         <v>PubMed:28252957</v>
       </c>
-      <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
       <c r="R24" s="3"/>
       <c r="S24" s="3"/>
@@ -24375,52 +24557,55 @@
       <c r="Z24" s="3"/>
       <c r="AA24" s="3"/>
       <c r="AB24" s="3"/>
-    </row>
-    <row r="25" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AC24" s="3"/>
+    </row>
+    <row r="25" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="20" t="s">
         <v>73</v>
       </c>
       <c r="B25" s="20" t="s">
+        <v>7626</v>
+      </c>
+      <c r="C25" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="20"/>
       <c r="D25" s="20"/>
-      <c r="E25" s="20" t="s">
+      <c r="E25" s="20"/>
+      <c r="F25" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="F25" s="20" t="s">
+      <c r="G25" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="G25" s="20" t="s">
+      <c r="H25" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="H25" s="20" t="s">
+      <c r="I25" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="I25" s="20">
+      <c r="J25" s="38">
         <v>28252957</v>
       </c>
-      <c r="J25" s="20" t="s">
+      <c r="K25" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="K25" t="s">
-        <v>7578</v>
-      </c>
-      <c r="L25" s="20" t="b">
+      <c r="L25" t="s">
+        <v>7573</v>
+      </c>
+      <c r="M25" s="20" t="b">
         <v>0</v>
       </c>
-      <c r="M25" s="18">
+      <c r="N25" s="18">
         <f t="shared" si="0"/>
         <v>256</v>
       </c>
-      <c r="N25" s="20" t="s">
+      <c r="O25" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="O25" s="18" t="str">
-        <f>Library!$H25&amp;":"&amp;Library!$I25</f>
+      <c r="P25" s="18" t="str">
+        <f>Library!$I25&amp;":"&amp;Library!$J25</f>
         <v>PubMed:28252957</v>
       </c>
-      <c r="P25" s="3"/>
       <c r="Q25" s="3"/>
       <c r="R25" s="3"/>
       <c r="S25" s="3"/>
@@ -24433,52 +24618,55 @@
       <c r="Z25" s="3"/>
       <c r="AA25" s="3"/>
       <c r="AB25" s="3"/>
-    </row>
-    <row r="26" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AC25" s="3"/>
+    </row>
+    <row r="26" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="20" t="s">
         <v>78</v>
       </c>
       <c r="B26" s="20" t="s">
+        <v>7626</v>
+      </c>
+      <c r="C26" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="C26" s="20"/>
       <c r="D26" s="20"/>
-      <c r="E26" s="20" t="s">
+      <c r="E26" s="20"/>
+      <c r="F26" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="F26" s="20" t="s">
+      <c r="G26" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="G26" s="20" t="s">
+      <c r="H26" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="H26" s="20" t="s">
+      <c r="I26" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="I26" s="20">
+      <c r="J26" s="38">
         <v>28252957</v>
       </c>
-      <c r="J26" s="20" t="s">
+      <c r="K26" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="K26" s="34" t="s">
-        <v>7578</v>
-      </c>
-      <c r="L26" s="20" t="b">
+      <c r="L26" s="34" t="s">
+        <v>7573</v>
+      </c>
+      <c r="M26" s="20" t="b">
         <v>0</v>
       </c>
-      <c r="M26" s="18">
+      <c r="N26" s="18">
         <f t="shared" si="0"/>
         <v>171</v>
       </c>
-      <c r="N26" s="20" t="s">
+      <c r="O26" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="O26" s="18" t="str">
-        <f>Library!$H26&amp;":"&amp;Library!$I26</f>
+      <c r="P26" s="18" t="str">
+        <f>Library!$I26&amp;":"&amp;Library!$J26</f>
         <v>PubMed:28252957</v>
       </c>
-      <c r="P26" s="3"/>
       <c r="Q26" s="3"/>
       <c r="R26" s="3"/>
       <c r="S26" s="3"/>
@@ -24491,52 +24679,55 @@
       <c r="Z26" s="3"/>
       <c r="AA26" s="3"/>
       <c r="AB26" s="3"/>
-    </row>
-    <row r="27" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AC26" s="3"/>
+    </row>
+    <row r="27" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="20" t="s">
         <v>82</v>
       </c>
       <c r="B27" s="20" t="s">
+        <v>7626</v>
+      </c>
+      <c r="C27" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="C27" s="20"/>
       <c r="D27" s="20"/>
-      <c r="E27" s="20" t="s">
+      <c r="E27" s="20"/>
+      <c r="F27" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="F27" s="20" t="s">
+      <c r="G27" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="G27" s="20" t="s">
+      <c r="H27" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="H27" s="20" t="s">
+      <c r="I27" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="I27" s="20">
+      <c r="J27" s="38">
         <v>28252957</v>
       </c>
-      <c r="J27" s="20" t="s">
+      <c r="K27" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="K27" t="s">
-        <v>7578</v>
-      </c>
-      <c r="L27" s="20" t="b">
+      <c r="L27" t="s">
+        <v>7573</v>
+      </c>
+      <c r="M27" s="20" t="b">
         <v>0</v>
       </c>
-      <c r="M27" s="18">
+      <c r="N27" s="18">
         <f t="shared" si="0"/>
         <v>228</v>
       </c>
-      <c r="N27" s="20" t="s">
+      <c r="O27" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="O27" s="18" t="str">
-        <f>Library!$H27&amp;":"&amp;Library!$I27</f>
+      <c r="P27" s="18" t="str">
+        <f>Library!$I27&amp;":"&amp;Library!$J27</f>
         <v>PubMed:28252957</v>
       </c>
-      <c r="P27" s="3"/>
       <c r="Q27" s="3"/>
       <c r="R27" s="3"/>
       <c r="S27" s="3"/>
@@ -24549,549 +24740,589 @@
       <c r="Z27" s="3"/>
       <c r="AA27" s="3"/>
       <c r="AB27" s="3"/>
-    </row>
-    <row r="28" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="AC27" s="3"/>
+    </row>
+    <row r="28" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="20" t="s">
         <v>86</v>
       </c>
       <c r="B28" s="20" t="s">
+        <v>7626</v>
+      </c>
+      <c r="C28" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="C28" s="20"/>
       <c r="D28" s="20"/>
       <c r="E28" s="20"/>
-      <c r="F28" s="20" t="s">
+      <c r="F28" s="20"/>
+      <c r="G28" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="G28" s="20" t="s">
+      <c r="H28" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="H28" s="20" t="s">
+      <c r="I28" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="I28" s="20">
+      <c r="J28" s="38">
         <v>28252957</v>
       </c>
-      <c r="J28" s="20"/>
-      <c r="K28" t="s">
-        <v>7578</v>
-      </c>
-      <c r="L28" s="20" t="b">
+      <c r="K28" s="20"/>
+      <c r="L28" t="s">
+        <v>7573</v>
+      </c>
+      <c r="M28" s="20" t="b">
         <v>0</v>
       </c>
-      <c r="M28" s="18">
+      <c r="N28" s="18">
         <f t="shared" si="0"/>
         <v>231</v>
       </c>
-      <c r="N28" s="20" t="s">
+      <c r="O28" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="O28" s="18" t="str">
-        <f>Library!$H28&amp;":"&amp;Library!$I28</f>
+      <c r="P28" s="18" t="str">
+        <f>Library!$I28&amp;":"&amp;Library!$J28</f>
         <v>PubMed:28252957</v>
       </c>
     </row>
-    <row r="29" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="20" t="s">
         <v>90</v>
       </c>
       <c r="B29" s="20" t="s">
+        <v>7626</v>
+      </c>
+      <c r="C29" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="C29" s="20"/>
       <c r="D29" s="20"/>
       <c r="E29" s="20"/>
       <c r="F29" s="20"/>
-      <c r="G29" s="20" t="s">
+      <c r="G29" s="20"/>
+      <c r="H29" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="H29" s="20" t="s">
+      <c r="I29" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="I29" s="20">
+      <c r="J29" s="38">
         <v>28252957</v>
       </c>
-      <c r="J29" s="20"/>
-      <c r="K29" t="s">
-        <v>7578</v>
-      </c>
-      <c r="L29" s="20" t="b">
+      <c r="K29" s="20"/>
+      <c r="L29" t="s">
+        <v>7573</v>
+      </c>
+      <c r="M29" s="20" t="b">
         <v>0</v>
       </c>
-      <c r="M29" s="18">
+      <c r="N29" s="18">
         <f t="shared" si="0"/>
         <v>225</v>
       </c>
-      <c r="N29" s="20" t="s">
+      <c r="O29" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="O29" s="18" t="str">
-        <f>Library!$H29&amp;":"&amp;Library!$I29</f>
+      <c r="P29" s="18" t="str">
+        <f>Library!$I29&amp;":"&amp;Library!$J29</f>
         <v>PubMed:28252957</v>
       </c>
     </row>
-    <row r="30" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="20" t="s">
         <v>93</v>
       </c>
       <c r="B30" s="20" t="s">
+        <v>7626</v>
+      </c>
+      <c r="C30" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="C30" s="20"/>
       <c r="D30" s="20"/>
       <c r="E30" s="20"/>
       <c r="F30" s="20"/>
-      <c r="G30" s="20" t="s">
+      <c r="G30" s="20"/>
+      <c r="H30" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="H30" s="20" t="s">
+      <c r="I30" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="I30" s="20">
+      <c r="J30" s="38">
         <v>28252957</v>
       </c>
-      <c r="J30" s="20"/>
-      <c r="K30" t="s">
-        <v>7578</v>
-      </c>
-      <c r="L30" s="20" t="b">
+      <c r="K30" s="20"/>
+      <c r="L30" t="s">
+        <v>7573</v>
+      </c>
+      <c r="M30" s="20" t="b">
         <v>0</v>
       </c>
-      <c r="M30" s="18">
+      <c r="N30" s="18">
         <f t="shared" si="0"/>
         <v>225</v>
       </c>
-      <c r="N30" s="20" t="s">
+      <c r="O30" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="O30" s="18" t="str">
-        <f>Library!$H30&amp;":"&amp;Library!$I30</f>
+      <c r="P30" s="18" t="str">
+        <f>Library!$I30&amp;":"&amp;Library!$J30</f>
         <v>PubMed:28252957</v>
       </c>
     </row>
-    <row r="31" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="20" t="s">
         <v>96</v>
       </c>
       <c r="B31" s="20" t="s">
+        <v>7626</v>
+      </c>
+      <c r="C31" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="C31" s="20"/>
       <c r="D31" s="20"/>
       <c r="E31" s="20"/>
       <c r="F31" s="20"/>
-      <c r="G31" s="20" t="s">
+      <c r="G31" s="20"/>
+      <c r="H31" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="H31" s="20" t="s">
+      <c r="I31" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="I31" s="20">
+      <c r="J31" s="38">
         <v>28252957</v>
       </c>
-      <c r="J31" s="20"/>
-      <c r="K31" t="s">
-        <v>7578</v>
-      </c>
-      <c r="L31" s="20" t="b">
+      <c r="K31" s="20"/>
+      <c r="L31" t="s">
+        <v>7573</v>
+      </c>
+      <c r="M31" s="20" t="b">
         <v>0</v>
       </c>
-      <c r="M31" s="18">
+      <c r="N31" s="18">
         <f t="shared" si="0"/>
         <v>219</v>
       </c>
-      <c r="N31" s="20" t="s">
+      <c r="O31" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="O31" s="18" t="str">
-        <f>Library!$H31&amp;":"&amp;Library!$I31</f>
+      <c r="P31" s="18" t="str">
+        <f>Library!$I31&amp;":"&amp;Library!$J31</f>
         <v>PubMed:28252957</v>
       </c>
     </row>
-    <row r="32" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:29" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="20" t="s">
         <v>99</v>
       </c>
       <c r="B32" s="20" t="s">
+        <v>7626</v>
+      </c>
+      <c r="C32" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="C32" s="20"/>
       <c r="D32" s="20"/>
       <c r="E32" s="20"/>
       <c r="F32" s="20"/>
-      <c r="G32" s="20" t="s">
-        <v>100</v>
-      </c>
+      <c r="G32" s="20"/>
       <c r="H32" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="I32" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="I32" s="20">
+      <c r="J32" s="38">
         <v>28252957</v>
       </c>
-      <c r="J32" s="20"/>
-      <c r="K32" t="s">
-        <v>7578</v>
-      </c>
-      <c r="L32" s="20" t="b">
+      <c r="K32" s="20"/>
+      <c r="L32" t="s">
+        <v>7573</v>
+      </c>
+      <c r="M32" s="20" t="b">
         <v>0</v>
       </c>
-      <c r="M32" s="18">
+      <c r="N32" s="18">
         <f t="shared" si="0"/>
         <v>228</v>
       </c>
-      <c r="N32" s="20" t="s">
+      <c r="O32" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="O32" s="18" t="str">
-        <f>Library!$H32&amp;":"&amp;Library!$I32</f>
+      <c r="P32" s="18" t="str">
+        <f>Library!$I32&amp;":"&amp;Library!$J32</f>
         <v>PubMed:28252957</v>
       </c>
     </row>
-    <row r="33" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="20" t="s">
         <v>102</v>
       </c>
       <c r="B33" s="20" t="s">
+        <v>7626</v>
+      </c>
+      <c r="C33" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="C33" s="20"/>
       <c r="D33" s="20"/>
       <c r="E33" s="20"/>
       <c r="F33" s="20"/>
-      <c r="G33" s="20" t="s">
+      <c r="G33" s="20"/>
+      <c r="H33" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="H33" s="20" t="s">
+      <c r="I33" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="I33" s="20">
+      <c r="J33" s="38">
         <v>28252957</v>
       </c>
-      <c r="J33" s="20"/>
-      <c r="K33" t="s">
-        <v>7578</v>
-      </c>
-      <c r="L33" s="20" t="b">
+      <c r="K33" s="20"/>
+      <c r="L33" t="s">
+        <v>7573</v>
+      </c>
+      <c r="M33" s="20" t="b">
         <v>0</v>
       </c>
-      <c r="M33" s="18">
+      <c r="N33" s="18">
         <f t="shared" si="0"/>
         <v>249</v>
       </c>
-      <c r="N33" s="20" t="s">
+      <c r="O33" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="O33" s="18" t="str">
-        <f>Library!$H33&amp;":"&amp;Library!$I33</f>
+      <c r="P33" s="18" t="str">
+        <f>Library!$I33&amp;":"&amp;Library!$J33</f>
         <v>PubMed:28252957</v>
       </c>
     </row>
-    <row r="34" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="20" t="s">
         <v>105</v>
       </c>
       <c r="B34" s="20" t="s">
+        <v>7626</v>
+      </c>
+      <c r="C34" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="C34" s="20"/>
       <c r="D34" s="20"/>
-      <c r="E34" s="20" t="s">
+      <c r="E34" s="20"/>
+      <c r="F34" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="F34" s="20" t="s">
+      <c r="G34" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="G34" s="20" t="s">
+      <c r="H34" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="H34" s="20" t="s">
+      <c r="I34" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="I34" s="20">
+      <c r="J34" s="38">
         <v>28252957</v>
       </c>
-      <c r="J34" s="20" t="s">
+      <c r="K34" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="K34" t="s">
-        <v>7578</v>
-      </c>
-      <c r="L34" s="20" t="b">
+      <c r="L34" t="s">
+        <v>7573</v>
+      </c>
+      <c r="M34" s="20" t="b">
         <v>1</v>
       </c>
-      <c r="M34" s="18">
+      <c r="N34" s="18">
         <f t="shared" si="0"/>
         <v>717</v>
       </c>
-      <c r="N34" s="20" t="s">
+      <c r="O34" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="O34" s="18" t="str">
-        <f>Library!$H34&amp;":"&amp;Library!$I34</f>
+      <c r="P34" s="18" t="str">
+        <f>Library!$I34&amp;":"&amp;Library!$J34</f>
         <v>PubMed:28252957</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="20" t="s">
         <v>111</v>
       </c>
       <c r="B35" s="20" t="s">
+        <v>7626</v>
+      </c>
+      <c r="C35" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="C35" s="20"/>
       <c r="D35" s="20"/>
-      <c r="E35" s="20" t="s">
+      <c r="E35" s="20"/>
+      <c r="F35" s="20" t="s">
         <v>107</v>
       </c>
-      <c r="F35" s="20" t="s">
+      <c r="G35" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="G35" s="20" t="s">
+      <c r="H35" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="H35" s="20" t="s">
+      <c r="I35" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="I35" s="20">
+      <c r="J35" s="38">
         <v>28252957</v>
       </c>
-      <c r="J35" s="20" t="s">
-        <v>7577</v>
-      </c>
-      <c r="K35" t="s">
-        <v>7578</v>
-      </c>
-      <c r="L35" s="20" t="b">
+      <c r="K35" s="20" t="s">
+        <v>7572</v>
+      </c>
+      <c r="L35" t="s">
+        <v>7573</v>
+      </c>
+      <c r="M35" s="20" t="b">
         <v>0</v>
       </c>
-      <c r="M35" s="18">
+      <c r="N35" s="18">
         <f t="shared" si="0"/>
         <v>738</v>
       </c>
-      <c r="N35" s="20" t="s">
+      <c r="O35" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="O35" s="18" t="str">
-        <f>Library!$H35&amp;":"&amp;Library!$I35</f>
+      <c r="P35" s="18" t="str">
+        <f>Library!$I35&amp;":"&amp;Library!$J35</f>
         <v>PubMed:28252957</v>
       </c>
     </row>
-    <row r="36" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="20" t="s">
         <v>114</v>
       </c>
       <c r="B36" s="20" t="s">
+        <v>7626</v>
+      </c>
+      <c r="C36" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="C36" s="20"/>
       <c r="D36" s="20"/>
-      <c r="E36" s="20" t="s">
+      <c r="E36" s="20"/>
+      <c r="F36" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="F36" s="20" t="s">
+      <c r="G36" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="G36" s="20" t="s">
+      <c r="H36" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="H36" s="20" t="s">
+      <c r="I36" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="I36" s="20">
+      <c r="J36" s="38">
         <v>28252957</v>
       </c>
-      <c r="J36" s="20" t="s">
+      <c r="K36" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="K36" t="s">
-        <v>7578</v>
-      </c>
-      <c r="L36" s="20" t="b">
+      <c r="L36" t="s">
+        <v>7573</v>
+      </c>
+      <c r="M36" s="20" t="b">
         <v>0</v>
       </c>
-      <c r="M36" s="18">
+      <c r="N36" s="18">
         <f t="shared" si="0"/>
         <v>714</v>
       </c>
-      <c r="N36" s="20" t="s">
+      <c r="O36" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="O36" s="18" t="str">
-        <f>Library!$H36&amp;":"&amp;Library!$I36</f>
+      <c r="P36" s="18" t="str">
+        <f>Library!$I36&amp;":"&amp;Library!$J36</f>
         <v>PubMed:28252957</v>
       </c>
     </row>
-    <row r="37" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="20" t="s">
         <v>117</v>
       </c>
       <c r="B37" s="20" t="s">
+        <v>7626</v>
+      </c>
+      <c r="C37" s="20" t="s">
         <v>106</v>
       </c>
-      <c r="C37" s="20"/>
       <c r="D37" s="20"/>
-      <c r="E37" s="20" t="s">
+      <c r="E37" s="20"/>
+      <c r="F37" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="F37" s="20" t="s">
+      <c r="G37" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="G37" s="20" t="s">
+      <c r="H37" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="H37" s="20" t="s">
+      <c r="I37" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="I37" s="20">
+      <c r="J37" s="38">
         <v>28252957</v>
       </c>
-      <c r="J37" s="20" t="s">
-        <v>7577</v>
-      </c>
-      <c r="K37" t="s">
-        <v>7578</v>
-      </c>
-      <c r="L37" s="20" t="b">
+      <c r="K37" s="20" t="s">
+        <v>7572</v>
+      </c>
+      <c r="L37" t="s">
+        <v>7573</v>
+      </c>
+      <c r="M37" s="20" t="b">
         <v>0</v>
       </c>
-      <c r="M37" s="18">
+      <c r="N37" s="18">
         <f t="shared" si="0"/>
         <v>735</v>
       </c>
-      <c r="N37" s="20" t="s">
+      <c r="O37" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="O37" s="18" t="str">
-        <f>Library!$H37&amp;":"&amp;Library!$I37</f>
+      <c r="P37" s="18" t="str">
+        <f>Library!$I37&amp;":"&amp;Library!$J37</f>
         <v>PubMed:28252957</v>
       </c>
     </row>
-    <row r="38" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="20" t="s">
         <v>119</v>
       </c>
       <c r="B38" s="20" t="s">
+        <v>7626</v>
+      </c>
+      <c r="C38" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="C38" s="20"/>
       <c r="D38" s="20"/>
       <c r="E38" s="20"/>
-      <c r="F38" s="20" t="s">
+      <c r="F38" s="20"/>
+      <c r="G38" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="G38" s="20" t="s">
+      <c r="H38" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="H38" s="20" t="s">
+      <c r="I38" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="I38" s="20">
+      <c r="J38" s="38">
         <v>28252957</v>
       </c>
-      <c r="J38" t="s">
-        <v>7578</v>
-      </c>
       <c r="K38" t="s">
-        <v>7578</v>
-      </c>
-      <c r="L38" s="20" t="b">
+        <v>7573</v>
+      </c>
+      <c r="L38" t="s">
+        <v>7573</v>
+      </c>
+      <c r="M38" s="20" t="b">
         <v>0</v>
       </c>
-      <c r="M38" s="18">
+      <c r="N38" s="18">
         <f t="shared" si="0"/>
         <v>247</v>
       </c>
-      <c r="N38" s="20" t="s">
+      <c r="O38" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="O38" s="18" t="str">
-        <f>Library!$H38&amp;":"&amp;Library!$I38</f>
+      <c r="P38" s="18" t="str">
+        <f>Library!$I38&amp;":"&amp;Library!$J38</f>
         <v>PubMed:28252957</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="20" t="s">
         <v>122</v>
       </c>
       <c r="B39" s="20" t="s">
+        <v>7626</v>
+      </c>
+      <c r="C39" s="20" t="s">
         <v>123</v>
       </c>
-      <c r="C39" s="20"/>
       <c r="D39" s="20"/>
-      <c r="E39" s="20" t="s">
+      <c r="E39" s="20"/>
+      <c r="F39" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="F39" s="20" t="s">
+      <c r="G39" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="G39" s="20" t="s">
+      <c r="H39" s="20" t="s">
         <v>124</v>
       </c>
-      <c r="H39" s="20" t="s">
+      <c r="I39" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="I39" s="20">
+      <c r="J39" s="38">
         <v>28252957</v>
       </c>
-      <c r="J39" s="20"/>
-      <c r="K39" t="s">
-        <v>7578</v>
-      </c>
-      <c r="L39" s="20" t="b">
+      <c r="K39" s="20"/>
+      <c r="L39" t="s">
+        <v>7573</v>
+      </c>
+      <c r="M39" s="20" t="b">
         <v>0</v>
       </c>
-      <c r="M39" s="18">
+      <c r="N39" s="18">
         <f t="shared" si="0"/>
         <v>187</v>
       </c>
-      <c r="N39" s="20" t="s">
+      <c r="O39" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="O39" s="18" t="str">
-        <f>Library!$H39&amp;":"&amp;Library!$I39</f>
+      <c r="P39" s="18" t="str">
+        <f>Library!$I39&amp;":"&amp;Library!$J39</f>
         <v>PubMed:28252957</v>
       </c>
     </row>
-    <row r="40" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="20" t="s">
         <v>126</v>
       </c>
       <c r="B40" s="20" t="s">
+        <v>7626</v>
+      </c>
+      <c r="C40" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="C40" s="20"/>
       <c r="D40" s="20"/>
       <c r="E40" s="20"/>
-      <c r="F40" s="20" t="s">
+      <c r="F40" s="20"/>
+      <c r="G40" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="G40" s="20" t="s">
+      <c r="H40" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="H40" s="20" t="s">
+      <c r="I40" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="I40" s="20">
+      <c r="J40" s="38">
         <v>28252957</v>
       </c>
-      <c r="J40" t="s">
-        <v>7578</v>
-      </c>
       <c r="K40" t="s">
-        <v>7578</v>
-      </c>
-      <c r="L40" s="20" t="b">
+        <v>7573</v>
+      </c>
+      <c r="L40" t="s">
+        <v>7573</v>
+      </c>
+      <c r="M40" s="20" t="b">
         <v>0</v>
       </c>
-      <c r="M40" s="18">
+      <c r="N40" s="18">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="N40" s="20" t="s">
-        <v>7579</v>
-      </c>
-      <c r="O40" s="18" t="str">
-        <f>Library!$H40&amp;":"&amp;Library!$I40</f>
+      <c r="O40" s="30" t="s">
+        <v>7574</v>
+      </c>
+      <c r="P40" s="18" t="str">
+        <f>Library!$I40&amp;":"&amp;Library!$J40</f>
         <v>PubMed:28252957</v>
       </c>
     </row>
@@ -25404,25 +25635,22 @@
   <mergeCells count="1">
     <mergeCell ref="A11:F11"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="O40" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>data_source!$B$2:$B$11</xm:f>
           </x14:formula1>
-          <xm:sqref>H20:H40</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>role_terms!$B$2:$B$2518</xm:f>
-          </x14:formula1>
-          <xm:sqref>B20:B40</xm:sqref>
+          <xm:sqref>I20:I40</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
           <x14:formula1>
@@ -25434,19 +25662,31 @@
           <x14:formula1>
             <xm:f>Sequence_alteration_terms!$A$2:$A$19</xm:f>
           </x14:formula1>
-          <xm:sqref>F20:F40</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>role_terms!$F$2:$F$3</xm:f>
-          </x14:formula1>
-          <xm:sqref>L20:L40</xm:sqref>
+          <xm:sqref>G20:G40</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'Organism Terms'!$A$2:$A$32</xm:f>
           </x14:formula1>
-          <xm:sqref>J20:K40</xm:sqref>
+          <xm:sqref>K20:L40</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Object_Types!$A$2:$A$35</xm:f>
+          </x14:formula1>
+          <xm:sqref>B20:B40</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>role_terms!$B$2:$B$2518</xm:f>
+          </x14:formula1>
+          <xm:sqref>C20:C40</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>circular_types!$A$2:$A$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>M20:M40</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -25459,10 +25699,285 @@
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
+  <dimension ref="A1:O30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A1" s="39" t="s">
+        <v>7654</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>7627</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7628</v>
+      </c>
+      <c r="I2" t="s">
+        <v>7628</v>
+      </c>
+      <c r="L2" t="s">
+        <v>7628</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>7629</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7628</v>
+      </c>
+      <c r="I3" t="s">
+        <v>7628</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>7630</v>
+      </c>
+      <c r="F4" t="s">
+        <v>7628</v>
+      </c>
+      <c r="I4" t="s">
+        <v>7628</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>7631</v>
+      </c>
+      <c r="F5" t="s">
+        <v>7628</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>7632</v>
+      </c>
+      <c r="F6" t="s">
+        <v>7628</v>
+      </c>
+      <c r="I6" t="s">
+        <v>7628</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>7633</v>
+      </c>
+      <c r="F7" t="s">
+        <v>7628</v>
+      </c>
+      <c r="I7" t="s">
+        <v>7628</v>
+      </c>
+      <c r="L7" t="s">
+        <v>7628</v>
+      </c>
+      <c r="O7" t="s">
+        <v>7628</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>7624</v>
+      </c>
+      <c r="F8" t="s">
+        <v>7628</v>
+      </c>
+      <c r="I8" t="s">
+        <v>7628</v>
+      </c>
+      <c r="L8" t="s">
+        <v>7628</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>7626</v>
+      </c>
+      <c r="F9" t="s">
+        <v>7628</v>
+      </c>
+      <c r="I9" t="s">
+        <v>7628</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>7634</v>
+      </c>
+      <c r="F10" t="s">
+        <v>7628</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>7635</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>7636</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>7637</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>7638</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>7639</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>7640</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>7641</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>7642</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>7643</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>7644</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>7645</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>7646</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>7647</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>7648</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>7649</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>7650</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>7651</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>7652</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>7653</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="D3:D35">
+    <sortCondition ref="D3"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="8"/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="40" t="s">
+        <v>7657</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>7658</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="8"/>
+  </sheetPr>
   <dimension ref="A1:M2535"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="F1" sqref="F1:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3046875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -25489,9 +26004,6 @@
         <v>131</v>
       </c>
       <c r="E1" s="21"/>
-      <c r="F1" s="21" t="s">
-        <v>132</v>
-      </c>
       <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -25508,9 +26020,6 @@
         <v>134</v>
       </c>
       <c r="E2" s="3"/>
-      <c r="F2" s="3" t="b">
-        <v>1</v>
-      </c>
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -25527,9 +26036,6 @@
         <v>136</v>
       </c>
       <c r="E3" s="3"/>
-      <c r="F3" s="3" t="b">
-        <v>0</v>
-      </c>
       <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -68008,7 +68514,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8"/>
@@ -68059,7 +68565,7 @@
         <v>7468</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7587</v>
+        <v>7582</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
@@ -68081,7 +68587,7 @@
         <v>7469</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>7588</v>
+        <v>7583</v>
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -68101,7 +68607,7 @@
         <v>7470</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>7589</v>
+        <v>7584</v>
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
@@ -68121,7 +68627,7 @@
         <v>7471</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>7590</v>
+        <v>7585</v>
       </c>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
@@ -68141,7 +68647,7 @@
         <v>7472</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>7591</v>
+        <v>7586</v>
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
@@ -68161,7 +68667,7 @@
         <v>7473</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>7592</v>
+        <v>7587</v>
       </c>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
@@ -68181,7 +68687,7 @@
         <v>7474</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>7593</v>
+        <v>7588</v>
       </c>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
@@ -68201,7 +68707,7 @@
         <v>7475</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>7594</v>
+        <v>7589</v>
       </c>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
@@ -68221,7 +68727,7 @@
         <v>7476</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>7595</v>
+        <v>7590</v>
       </c>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
@@ -68241,7 +68747,7 @@
         <v>7477</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>7596</v>
+        <v>7591</v>
       </c>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
@@ -68261,7 +68767,7 @@
         <v>7478</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>7597</v>
+        <v>7592</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
@@ -68269,7 +68775,7 @@
         <v>7479</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>7598</v>
+        <v>7593</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
@@ -68277,7 +68783,7 @@
         <v>7480</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>7599</v>
+        <v>7594</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
@@ -68285,7 +68791,7 @@
         <v>7481</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>7600</v>
+        <v>7595</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="15.5" x14ac:dyDescent="0.35">
@@ -68293,7 +68799,7 @@
         <v>7482</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>7601</v>
+        <v>7596</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -68301,7 +68807,7 @@
         <v>7483</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>7602</v>
+        <v>7597</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -68309,7 +68815,7 @@
         <v>7484</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>7603</v>
+        <v>7598</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -68317,7 +68823,7 @@
         <v>7485</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>7604</v>
+        <v>7599</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -68325,7 +68831,7 @@
         <v>7486</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>7605</v>
+        <v>7600</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -68333,7 +68839,7 @@
         <v>7487</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>7606</v>
+        <v>7601</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -68341,7 +68847,7 @@
         <v>7488</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>7607</v>
+        <v>7602</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -68349,7 +68855,7 @@
         <v>7489</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>7608</v>
+        <v>7603</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -68357,7 +68863,7 @@
         <v>7490</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>7609</v>
+        <v>7604</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -68365,7 +68871,7 @@
         <v>64</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>7610</v>
+        <v>7605</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -68373,7 +68879,7 @@
         <v>7491</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>7611</v>
+        <v>7606</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -68381,7 +68887,7 @@
         <v>7492</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>7612</v>
+        <v>7607</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -68389,7 +68895,7 @@
         <v>7493</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>7613</v>
+        <v>7608</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
@@ -68397,23 +68903,23 @@
         <v>18</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>7614</v>
+        <v>7609</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>7578</v>
+        <v>7573</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>7615</v>
+        <v>7610</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" s="35" t="s">
-        <v>7577</v>
+        <v>7572</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>7616</v>
+        <v>7611</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -69222,7 +69728,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8"/>
@@ -69328,7 +69834,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8"/>
@@ -69336,7 +69842,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3046875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -69399,54 +69905,54 @@
       <c r="C3" s="27" t="s">
         <v>7521</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="42" t="s">
+        <v>7663</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>7522</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>7523</v>
-      </c>
-      <c r="F3" s="27" t="s">
-        <v>7524</v>
+      <c r="F3" s="42" t="s">
+        <v>7662</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
+        <v>7523</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>7524</v>
+      </c>
+      <c r="C4" s="27" t="s">
         <v>7525</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="D4" s="27" t="s">
         <v>7526</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="E4" s="14" t="s">
         <v>7527</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="F4" s="27" t="s">
         <v>7528</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>7529</v>
-      </c>
-      <c r="F4" s="27" t="s">
-        <v>7530</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
+        <v>7529</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>7530</v>
+      </c>
+      <c r="C5" s="27" t="s">
         <v>7531</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="D5" s="42" t="s">
+        <v>7660</v>
+      </c>
+      <c r="E5" s="14" t="s">
         <v>7532</v>
       </c>
-      <c r="C5" s="27" t="s">
-        <v>7533</v>
-      </c>
-      <c r="D5" s="27" t="s">
-        <v>7534</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>7535</v>
-      </c>
-      <c r="F5" s="27" t="s">
-        <v>7536</v>
+      <c r="F5" s="42" t="s">
+        <v>7661</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -69454,19 +69960,19 @@
         <v>16</v>
       </c>
       <c r="B6" s="14" t="s">
+        <v>7533</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>7534</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>7535</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>7536</v>
+      </c>
+      <c r="F6" s="27" t="s">
         <v>7537</v>
-      </c>
-      <c r="C6" s="27" t="s">
-        <v>7538</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>7539</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>7540</v>
-      </c>
-      <c r="F6" s="27" t="s">
-        <v>7541</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -69474,19 +69980,19 @@
         <v>7467</v>
       </c>
       <c r="B7" s="14" t="s">
+        <v>7538</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>7539</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>7540</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>7541</v>
+      </c>
+      <c r="F7" s="28" t="s">
         <v>7542</v>
-      </c>
-      <c r="C7" s="27" t="s">
-        <v>7543</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>7544</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>7545</v>
-      </c>
-      <c r="F7" s="28" t="s">
-        <v>7546</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -69557,21 +70063,22 @@
     <hyperlink ref="C7" r:id="rId15"/>
     <hyperlink ref="D7" r:id="rId16"/>
     <hyperlink ref="F7" r:id="rId17"/>
+    <hyperlink ref="D3" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="8"/>
   </sheetPr>
-  <dimension ref="A1:AD23"/>
+  <dimension ref="A1:AD24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.3046875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -69587,43 +70094,43 @@
   <sheetData>
     <row r="1" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
+        <v>7543</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>7544</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>7545</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>7577</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>7575</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>7579</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>7570</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>7546</v>
+      </c>
+      <c r="I1" s="21" t="s">
         <v>7547</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>7548</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="K1" s="21" t="s">
         <v>7549</v>
       </c>
-      <c r="D1" s="21" t="s">
-        <v>7582</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>7580</v>
-      </c>
-      <c r="F1" s="21" t="s">
-        <v>7584</v>
-      </c>
-      <c r="G1" s="31" t="s">
-        <v>7575</v>
-      </c>
-      <c r="H1" s="21" t="s">
+      <c r="L1" s="21" t="s">
         <v>7550</v>
       </c>
-      <c r="I1" s="21" t="s">
-        <v>7551</v>
-      </c>
-      <c r="J1" s="21" t="s">
-        <v>7552</v>
-      </c>
-      <c r="K1" s="21" t="s">
-        <v>7553</v>
-      </c>
-      <c r="L1" s="21" t="s">
-        <v>7554</v>
-      </c>
       <c r="M1" s="32" t="s">
-        <v>7576</v>
+        <v>7571</v>
       </c>
     </row>
     <row r="2" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -69631,16 +70138,16 @@
         <v>37</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7555</v>
+        <v>7551</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>7556</v>
+        <v>7552</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>7583</v>
+        <v>7578</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>7581</v>
+        <v>7576</v>
       </c>
       <c r="F2" s="35"/>
       <c r="G2" s="33" t="b">
@@ -69659,89 +70166,89 @@
     </row>
     <row r="3" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>7617</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>7556</v>
+        <v>7623</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>7625</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>7552</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>7583</v>
+        <v>7578</v>
       </c>
       <c r="E3" s="35" t="s">
-        <v>130</v>
-      </c>
-      <c r="F3" s="36" t="s">
-        <v>7585</v>
-      </c>
+        <v>7576</v>
+      </c>
+      <c r="F3" s="35"/>
       <c r="G3" s="33" t="b">
-        <v>1</v>
-      </c>
-      <c r="H3" s="33" t="b">
         <v>0</v>
       </c>
-      <c r="I3" s="3" t="b">
+      <c r="H3" s="20" t="b">
         <v>0</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="34" t="s">
-        <v>7573</v>
-      </c>
+      <c r="I3" s="20" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="34"/>
     </row>
     <row r="4" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="29" t="s">
-        <v>7624</v>
-      </c>
-      <c r="B4" s="20" t="s">
-        <v>7621</v>
-      </c>
-      <c r="C4" s="25" t="s">
-        <v>7559</v>
+        <v>38</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7612</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>7552</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>7622</v>
+        <v>7617</v>
       </c>
       <c r="E4" s="35" t="s">
-        <v>7581</v>
-      </c>
-      <c r="F4" s="35" t="s">
-        <v>7586</v>
+        <v>130</v>
+      </c>
+      <c r="F4" s="36" t="s">
+        <v>7580</v>
       </c>
       <c r="G4" s="33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" s="33" t="b">
         <v>0</v>
       </c>
-      <c r="I4" s="20" t="b">
+      <c r="I4" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="34"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="34" t="s">
+        <v>7568</v>
+      </c>
     </row>
     <row r="5" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="29" t="s">
-        <v>7619</v>
+        <v>7620</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>7621</v>
+        <v>7616</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>7559</v>
+        <v>7555</v>
       </c>
       <c r="D5" s="35" t="s">
-        <v>7622</v>
+        <v>7618</v>
       </c>
       <c r="E5" s="35" t="s">
+        <v>7576</v>
+      </c>
+      <c r="F5" s="35" t="s">
         <v>7581</v>
       </c>
-      <c r="F5" s="36"/>
       <c r="G5" s="33" t="b">
         <v>0</v>
       </c>
@@ -69754,124 +70261,124 @@
       <c r="J5" s="20"/>
       <c r="K5" s="20"/>
       <c r="L5" s="20"/>
-      <c r="M5" s="34" t="s">
-        <v>7573</v>
-      </c>
+      <c r="M5" s="34"/>
     </row>
     <row r="6" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>7558</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>7559</v>
+        <v>7614</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>7616</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>7555</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>7583</v>
+        <v>7618</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>7581</v>
-      </c>
-      <c r="F6" s="35"/>
+        <v>7576</v>
+      </c>
+      <c r="F6" s="36"/>
       <c r="G6" s="33" t="b">
         <v>0</v>
       </c>
-      <c r="H6" s="3" t="b">
+      <c r="H6" s="33" t="b">
         <v>0</v>
       </c>
-      <c r="I6" s="3" t="b">
+      <c r="I6" s="20" t="b">
         <v>0</v>
       </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="34"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="34" t="s">
+        <v>7568</v>
+      </c>
     </row>
     <row r="7" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="35" t="s">
-        <v>7560</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>7559</v>
+        <v>39</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>7554</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>7555</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>7583</v>
+        <v>7578</v>
       </c>
       <c r="E7" s="35" t="s">
-        <v>130</v>
+        <v>7576</v>
       </c>
       <c r="F7" s="35"/>
       <c r="G7" s="33" t="b">
         <v>0</v>
       </c>
       <c r="H7" s="3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="J7" s="3" t="s">
-        <v>7561</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>7562</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>7557</v>
-      </c>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
       <c r="M7" s="34"/>
     </row>
     <row r="8" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>7618</v>
+        <v>40</v>
+      </c>
+      <c r="B8" s="35" t="s">
+        <v>7556</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>7563</v>
+        <v>7555</v>
       </c>
       <c r="D8" s="35" t="s">
-        <v>7583</v>
+        <v>7578</v>
       </c>
       <c r="E8" s="35" t="s">
-        <v>7581</v>
+        <v>130</v>
       </c>
       <c r="F8" s="35"/>
       <c r="G8" s="33" t="b">
         <v>0</v>
       </c>
       <c r="H8" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
+      <c r="J8" s="3" t="s">
+        <v>7557</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>7558</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>7553</v>
+      </c>
       <c r="M8" s="34"/>
     </row>
     <row r="9" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>7564</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>7564</v>
+        <v>7613</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>7559</v>
       </c>
       <c r="D9" s="35" t="s">
-        <v>7583</v>
+        <v>7578</v>
       </c>
       <c r="E9" s="35" t="s">
-        <v>7564</v>
+        <v>7576</v>
       </c>
       <c r="F9" s="35"/>
       <c r="G9" s="33" t="b">
@@ -69883,23 +70390,26 @@
       <c r="I9" s="3" t="b">
         <v>0</v>
       </c>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
       <c r="M9" s="34"/>
     </row>
     <row r="10" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>7564</v>
+        <v>7560</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>7564</v>
+        <v>7560</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>7583</v>
+        <v>7578</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>7564</v>
+        <v>7560</v>
       </c>
       <c r="F10" s="35"/>
       <c r="G10" s="33" t="b">
@@ -69911,47 +70421,27 @@
       <c r="I10" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
       <c r="M10" s="34"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
-      <c r="S10" s="3"/>
-      <c r="T10" s="3"/>
-      <c r="U10" s="3"/>
-      <c r="V10" s="3"/>
-      <c r="W10" s="3"/>
-      <c r="X10" s="3"/>
-      <c r="Y10" s="3"/>
-      <c r="Z10" s="3"/>
-      <c r="AA10" s="3"/>
-      <c r="AB10" s="3"/>
-      <c r="AC10" s="3"/>
-      <c r="AD10" s="3"/>
     </row>
     <row r="11" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>7565</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>7559</v>
+        <v>7560</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>7560</v>
       </c>
       <c r="D11" s="35" t="s">
-        <v>7583</v>
+        <v>7578</v>
       </c>
       <c r="E11" s="35" t="s">
-        <v>130</v>
+        <v>7560</v>
       </c>
       <c r="F11" s="35"/>
       <c r="G11" s="33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11" s="3" t="b">
         <v>0</v>
@@ -69962,22 +70452,37 @@
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
-      <c r="M11" t="s">
-        <v>7574</v>
-      </c>
+      <c r="M11" s="34"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
+      <c r="AA11" s="3"/>
+      <c r="AB11" s="3"/>
+      <c r="AC11" s="3"/>
+      <c r="AD11" s="3"/>
     </row>
     <row r="12" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>7566</v>
-      </c>
-      <c r="C12" s="30" t="s">
-        <v>7559</v>
+        <v>7561</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>7555</v>
       </c>
       <c r="D12" s="35" t="s">
-        <v>7583</v>
+        <v>7578</v>
       </c>
       <c r="E12" s="35" t="s">
         <v>130</v>
@@ -69996,28 +70501,28 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" t="s">
-        <v>7574</v>
+        <v>7569</v>
       </c>
     </row>
     <row r="13" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13" s="37" t="s">
-        <v>7567</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>7556</v>
+        <v>45</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>7562</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>7555</v>
       </c>
       <c r="D13" s="35" t="s">
-        <v>7583</v>
+        <v>7578</v>
       </c>
       <c r="E13" s="35" t="s">
         <v>130</v>
       </c>
       <c r="F13" s="35"/>
       <c r="G13" s="33" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" s="3" t="b">
         <v>0</v>
@@ -70028,58 +70533,66 @@
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
-      <c r="M13" s="34"/>
+      <c r="M13" t="s">
+        <v>7569</v>
+      </c>
     </row>
     <row r="14" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>7564</v>
+        <v>46</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>7612</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>7564</v>
+        <v>7552</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>7583</v>
+        <v>7578</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>7564</v>
-      </c>
-      <c r="F14" s="35"/>
+        <v>130</v>
+      </c>
+      <c r="F14" s="36" t="s">
+        <v>7580</v>
+      </c>
       <c r="G14" s="33" t="b">
         <v>0</v>
       </c>
       <c r="H14" s="3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I14" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
+      <c r="J14" s="33" t="s">
+        <v>7659</v>
+      </c>
+      <c r="K14" s="33" t="s">
+        <v>7558</v>
+      </c>
+      <c r="L14" s="33" t="s">
+        <v>7553</v>
+      </c>
       <c r="M14" s="34"/>
     </row>
     <row r="15" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="29" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="37" t="s">
-        <v>7568</v>
+        <v>47</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>7560</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>7556</v>
+        <v>7560</v>
       </c>
       <c r="D15" s="35" t="s">
-        <v>7583</v>
+        <v>7578</v>
       </c>
       <c r="E15" s="35" t="s">
-        <v>7581</v>
-      </c>
-      <c r="F15" s="35" t="s">
-        <v>7586</v>
-      </c>
+        <v>7560</v>
+      </c>
+      <c r="F15" s="35"/>
       <c r="G15" s="33" t="b">
         <v>0</v>
       </c>
@@ -70096,66 +70609,99 @@
     </row>
     <row r="16" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>7569</v>
-      </c>
-      <c r="C16" s="35" t="s">
-        <v>7570</v>
+        <v>7563</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>7552</v>
       </c>
       <c r="D16" s="35" t="s">
-        <v>7583</v>
+        <v>7578</v>
       </c>
       <c r="E16" s="35" t="s">
-        <v>130</v>
-      </c>
-      <c r="F16" s="35"/>
+        <v>7576</v>
+      </c>
+      <c r="F16" s="35" t="s">
+        <v>7655</v>
+      </c>
       <c r="G16" s="33" t="b">
         <v>0</v>
       </c>
       <c r="H16" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" s="3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="34"/>
+    </row>
+    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="37" t="s">
+        <v>7564</v>
+      </c>
+      <c r="C17" s="35" t="s">
+        <v>7565</v>
+      </c>
+      <c r="D17" s="35" t="s">
+        <v>7578</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="F17" s="35"/>
+      <c r="G17" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="I16" s="3" t="b">
+      <c r="I17" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="J16" s="3" t="s">
-        <v>7571</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>7557</v>
-      </c>
-      <c r="L16" s="3" t="s">
-        <v>7572</v>
-      </c>
-      <c r="M16" s="34"/>
-    </row>
-    <row r="23" spans="8:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="3"/>
-      <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
-      <c r="N23" s="3"/>
-      <c r="O23" s="3"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
-      <c r="R23" s="3"/>
-      <c r="S23" s="3"/>
+      <c r="J17" s="3" t="s">
+        <v>7566</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>7553</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>7567</v>
+      </c>
+      <c r="M17" s="34"/>
+    </row>
+    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C6" r:id="rId1"/>
-    <hyperlink ref="C7" r:id="rId2"/>
-    <hyperlink ref="C8" r:id="rId3"/>
-    <hyperlink ref="C11" r:id="rId4"/>
-    <hyperlink ref="C12" r:id="rId5"/>
-    <hyperlink ref="C3" r:id="rId6"/>
-    <hyperlink ref="C5" r:id="rId7"/>
-    <hyperlink ref="C4" r:id="rId8"/>
-    <hyperlink ref="C16" r:id="rId9" display="https://wiki.synbiohub.org/wiki/Terms/synbiohub#"/>
+    <hyperlink ref="C7" r:id="rId1"/>
+    <hyperlink ref="C8" r:id="rId2"/>
+    <hyperlink ref="C9" r:id="rId3"/>
+    <hyperlink ref="C12" r:id="rId4"/>
+    <hyperlink ref="C13" r:id="rId5"/>
+    <hyperlink ref="C4" r:id="rId6"/>
+    <hyperlink ref="C6" r:id="rId7"/>
+    <hyperlink ref="C5" r:id="rId8"/>
+    <hyperlink ref="C17" r:id="rId9" display="https://wiki.synbiohub.org/wiki/Terms/synbiohub#"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId10"/>

</xml_diff>